<commit_message>
99% 2to3 tool converted Rest is minor modifications to module imports and string encoding Also update pinned environment
</commit_message>
<xml_diff>
--- a/spreadsheets/console.xlsx
+++ b/spreadsheets/console.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/msee/Projects/2020/SNAP-TB/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0677E1-7F0F-1443-9B3B-37B82E5621B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8475559-936A-3E41-9C40-F7E8528EA9BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="239">
   <si>
     <t>project_name</t>
   </si>
@@ -740,6 +740,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Test is 105</t>
   </si>
 </sst>
 </file>
@@ -1222,6 +1225,9 @@
         <v>3</v>
       </c>
       <c r="D5" s="2"/>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">

</xml_diff>